<commit_message>
fixing a series/movie error
</commit_message>
<xml_diff>
--- a/datasets/NetflixViewingHistory.xlsx
+++ b/datasets/NetflixViewingHistory.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tomi\SCHOOL\_EGYETEM\UvA\_STUDIES\4th semester\Data Processing\Final project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tomi\SCHOOL\_EGYETEM\UvA\_STUDIES\4th semester\Data Processing\Final project\sciprog-dp-uva\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BBAB5E-300D-401F-87D6-8ADCAD2C4F04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F06FC20-EF87-4729-8213-7AE04C9B3F03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6599,8 +6599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1343" workbookViewId="0">
-      <selection activeCell="A1363" sqref="A1363"/>
+    <sheetView tabSelected="1" topLeftCell="A562" workbookViewId="0">
+      <selection activeCell="A573" sqref="A573"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14756,7 +14756,7 @@
         <v>188</v>
       </c>
       <c r="D582" s="3" t="s">
-        <v>6</v>
+        <v>100</v>
       </c>
     </row>
     <row r="583" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>